<commit_message>
Actualizaci├│n autom├ítica de datos y commit
</commit_message>
<xml_diff>
--- a/establecimientos_pendientes.xlsx
+++ b/establecimientos_pendientes.xlsx
@@ -1258,7 +1258,7 @@
         <v>86</v>
       </c>
       <c r="D10">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -1294,7 +1294,7 @@
         <v>20</v>
       </c>
       <c r="P10">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Q10">
         <v>2024</v>
@@ -1534,7 +1534,7 @@
         <v>92</v>
       </c>
       <c r="D16">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1570,7 +1570,7 @@
         <v>7</v>
       </c>
       <c r="P16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Q16">
         <v>2024</v>
@@ -1590,7 +1590,7 @@
         <v>93</v>
       </c>
       <c r="D17">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E17">
         <v>23</v>
@@ -1626,7 +1626,7 @@
         <v>17</v>
       </c>
       <c r="P17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Q17">
         <v>2024</v>
@@ -4089,7 +4089,7 @@
         <v>144</v>
       </c>
       <c r="D68">
-        <v>14954</v>
+        <v>16590</v>
       </c>
       <c r="E68">
         <v>1573</v>
@@ -4119,7 +4119,7 @@
         <v>1544</v>
       </c>
       <c r="N68">
-        <v>420</v>
+        <v>2056</v>
       </c>
       <c r="Q68">
         <v>2024</v>

</xml_diff>